<commit_message>
initial madagascar data commit
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/blacklisted_words.xlsx
+++ b/mosip_master/xlsx/blacklisted_words.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji.Alluru\Desktop\Mosip\GitHub\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Country Details\Madagascar\MDG_Master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB32ECE0-CECA-46E6-A092-9C2F4A6617BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5499706E-EAB0-4A07-93CE-3D78D2A7C13F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>lang_code</t>
   </si>
@@ -38,27 +39,6 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>eng</t>
-  </si>
-  <si>
-    <t>shit</t>
-  </si>
-  <si>
-    <t>Blacklisted Word</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>damn</t>
-  </si>
-  <si>
-    <t>nigga</t>
-  </si>
-  <si>
-    <t>dammit</t>
-  </si>
-  <si>
     <t>fra</t>
   </si>
   <si>
@@ -69,51 +49,49 @@
   </si>
   <si>
     <t>bon sang</t>
-  </si>
-  <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>القرف</t>
-  </si>
-  <si>
-    <t>كلمة في القائمة السوداء</t>
-  </si>
-  <si>
-    <t>اللعنة</t>
-  </si>
-  <si>
-    <t>نيغا</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -122,17 +100,92 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9A9A9A"/>
       </bottom>
       <diagonal/>
     </border>
@@ -140,18 +193,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -187,7 +253,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -199,7 +265,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -246,6 +312,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -281,6 +364,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,22 +532,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CABD808-9163-4CF4-958E-2A97759329BE}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -456,12 +555,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" ht="22.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -470,133 +569,26 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13"/>
+      <c r="D3" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>